<commit_message>
further grooming and iterations over min and max aggregations. hopefully should be able to generalise lists
</commit_message>
<xml_diff>
--- a/Backend/app/datasets/app_sug_2.xlsx
+++ b/Backend/app/datasets/app_sug_2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Desktop/Projects/GlassByte/Diabetes/Backend/app/datasets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="8200" tabRatio="891" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="891" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MDI advice before planned ex" sheetId="1" r:id="rId1"/>
@@ -19,6 +24,9 @@
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="204">
   <si>
     <r>
       <rPr>
@@ -880,7 +888,7 @@
     <t>https://www.indi.ie/images/Breakfast_-_A_Great_Start_to_Your_Day.pdf</t>
   </si>
   <si>
-    <t>Intensity</t>
+    <t>BG</t>
   </si>
 </sst>
 </file>
@@ -1231,6 +1239,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1558,27 +1571,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="28.83203125" customWidth="1"/>
     <col min="6" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1610,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1614,7 +1627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>11</v>
@@ -1623,18 +1636,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="E5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1">
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1651,7 +1664,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1659,18 +1672,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="E9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E10" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -1687,7 +1700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1695,13 +1708,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="E13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1">
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
@@ -1709,7 +1722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1723,7 +1736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -1731,12 +1744,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E17" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1760,7 +1773,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="20" spans="1:22" ht="28">
+    <row r="20" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1777,7 +1790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1785,17 +1798,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="7" customFormat="1">
+    <row r="23" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E23" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="28">
+    <row r="24" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1812,7 +1825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D25" s="5" t="s">
         <v>11</v>
       </c>
@@ -1820,17 +1833,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="7" customFormat="1">
+    <row r="27" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E27" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="28">
+    <row r="28" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>6</v>
       </c>
@@ -1845,7 +1858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="28">
+    <row r="29" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -1860,12 +1873,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="3" customFormat="1">
+    <row r="30" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:1024" s="3" customFormat="1">
+    <row r="33" spans="1:1024" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>1</v>
       </c>
@@ -1880,7 +1893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:1024" ht="28">
+    <row r="34" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -1897,7 +1910,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:1024">
+    <row r="35" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
@@ -1905,17 +1918,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:1024">
+    <row r="36" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="E36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:1024">
+    <row r="37" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="E37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:1024">
+    <row r="38" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="D38" s="5" t="s">
         <v>37</v>
       </c>
@@ -1923,7 +1936,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1024" s="7" customFormat="1">
+    <row r="39" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D39" s="16" t="s">
         <v>37</v>
       </c>
@@ -1931,7 +1944,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1024">
+    <row r="40" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>35</v>
       </c>
@@ -1945,7 +1958,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:1024">
+    <row r="41" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>26</v>
       </c>
@@ -1953,13 +1966,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1024" s="7" customFormat="1">
+    <row r="42" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E42" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:1024" s="3" customFormat="1"/>
-    <row r="45" spans="1:1024" ht="28">
+    <row r="43" spans="1:1024" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:1024" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>35</v>
       </c>
@@ -1976,7 +1989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:1024">
+    <row r="46" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="D46" s="5" t="s">
         <v>11</v>
       </c>
@@ -1984,7 +1997,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1024">
+    <row r="47" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
         <v>43</v>
       </c>
@@ -4698,12 +4711,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:1024">
+    <row r="48" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="E48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D49" s="17" t="s">
         <v>37</v>
       </c>
@@ -4711,7 +4724,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D50" s="17" t="s">
         <v>37</v>
       </c>
@@ -4719,10 +4732,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D51" s="11"/>
     </row>
-    <row r="52" spans="1:5" s="18" customFormat="1" ht="28">
+    <row r="52" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>35</v>
       </c>
@@ -4737,7 +4750,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>35</v>
       </c>
@@ -4752,13 +4765,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="3" customFormat="1">
+    <row r="54" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="21" customFormat="1"/>
-    <row r="56" spans="1:5" s="23" customFormat="1">
+    <row r="55" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
         <v>1</v>
       </c>
@@ -4773,7 +4786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="21" customFormat="1">
+    <row r="57" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>45</v>
       </c>
@@ -4788,7 +4801,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="28">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>45</v>
       </c>
@@ -4803,7 +4816,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>49</v>
       </c>
@@ -4811,8 +4824,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1"/>
-    <row r="62" spans="1:5" s="21" customFormat="1" ht="28">
+    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:5" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>45</v>
       </c>
@@ -4827,7 +4840,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="28">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>45</v>
       </c>
@@ -4842,7 +4855,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="26"/>
       <c r="B64" t="s">
         <v>49</v>
@@ -4853,14 +4866,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="7" customFormat="1">
+    <row r="65" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E65" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="3" customFormat="1"/>
-    <row r="67" spans="1:5" ht="14.25" customHeight="1"/>
-    <row r="68" spans="1:5" s="29" customFormat="1">
+    <row r="66" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="27" t="s">
         <v>54</v>
       </c>
@@ -4872,11 +4885,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4884,11 +4892,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
@@ -4896,18 +4904,18 @@
     <col min="4" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15">
+    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>203</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -4933,7 +4941,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="31.5" customHeight="1">
+    <row r="3" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -4947,7 +4955,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>6</v>
       </c>
@@ -4957,7 +4965,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="7" customFormat="1">
+    <row r="5" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>6</v>
       </c>
@@ -4965,7 +4973,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>6</v>
       </c>
@@ -4979,7 +4987,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -4987,7 +4995,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
@@ -4995,7 +5003,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="7" customFormat="1">
+    <row r="9" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>6</v>
       </c>
@@ -5003,8 +5011,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="3" customFormat="1"/>
-    <row r="12" spans="1:21">
+    <row r="10" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -5035,7 +5043,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="30" customHeight="1">
+    <row r="13" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>35</v>
       </c>
@@ -5049,7 +5057,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -5057,7 +5065,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -5065,13 +5073,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="7" customFormat="1"/>
-    <row r="19" spans="1:22">
+    <row r="17" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -5102,7 +5110,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
     </row>
-    <row r="20" spans="1:22" s="21" customFormat="1">
+    <row r="20" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -5116,7 +5124,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="28">
+    <row r="21" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
         <v>45</v>
       </c>
@@ -5130,7 +5138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -5138,7 +5146,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -5146,13 +5154,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="7" customFormat="1"/>
-    <row r="26" spans="1:22" s="21" customFormat="1" ht="28">
+    <row r="25" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:22" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>45</v>
       </c>
@@ -5167,7 +5175,7 @@
       </c>
       <c r="F26" s="33"/>
     </row>
-    <row r="27" spans="1:22" ht="28">
+    <row r="27" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
         <v>45</v>
       </c>
@@ -5181,23 +5189,23 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C28" s="9"/>
       <c r="D28" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D29" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5224,11 +5232,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5236,11 +5239,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
@@ -5249,13 +5252,13 @@
     <col min="5" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15">
+    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:22" s="3" customFormat="1">
+    <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5272,7 +5275,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:22" ht="28">
+    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -5288,12 +5291,12 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D5" s="5" t="s">
         <v>76</v>
       </c>
@@ -5301,7 +5304,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="7" customFormat="1">
+    <row r="6" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D6" s="16" t="s">
         <v>78</v>
       </c>
@@ -5309,7 +5312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -5323,7 +5326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -5331,12 +5334,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D10" s="5" t="s">
         <v>81</v>
       </c>
@@ -5344,7 +5347,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="7" customFormat="1">
+    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D11" s="16" t="s">
         <v>78</v>
       </c>
@@ -5352,7 +5355,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5376,7 +5379,7 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
-    <row r="14" spans="1:22" ht="28">
+    <row r="14" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
         <v>6</v>
       </c>
@@ -5391,12 +5394,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D16" s="5" t="s">
         <v>76</v>
       </c>
@@ -5404,7 +5407,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="7" customFormat="1">
+    <row r="17" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D17" s="16" t="s">
         <v>78</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="28">
+    <row r="18" spans="1:24" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>6</v>
       </c>
@@ -5439,7 +5442,7 @@
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
     </row>
-    <row r="19" spans="1:24" ht="28">
+    <row r="19" spans="1:24" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>6</v>
       </c>
@@ -5454,7 +5457,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>26</v>
@@ -5475,7 +5478,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -5502,7 +5505,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:24" s="7" customFormat="1" ht="28">
+    <row r="24" spans="1:24" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
@@ -5524,7 +5527,7 @@
       <c r="W24" s="18"/>
       <c r="X24" s="18"/>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
         <v>88</v>
       </c>
@@ -5536,7 +5539,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -5547,7 +5550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -5558,7 +5561,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="3" customFormat="1">
+    <row r="28" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D28" s="17" t="s">
         <v>37</v>
       </c>
@@ -5566,7 +5569,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="7" customFormat="1">
+    <row r="29" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D29" s="16" t="s">
         <v>37</v>
       </c>
@@ -5574,7 +5577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
@@ -5588,7 +5591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>26</v>
       </c>
@@ -5596,12 +5599,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -5612,7 +5615,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -5623,8 +5626,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="7" customFormat="1"/>
-    <row r="37" spans="1:17" ht="28">
+    <row r="35" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:17" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
@@ -5639,12 +5642,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -5655,7 +5658,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -5666,7 +5669,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="21" customFormat="1">
+    <row r="41" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D41" s="17" t="s">
         <v>37</v>
       </c>
@@ -5674,7 +5677,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D42" s="17" t="s">
         <v>37</v>
       </c>
@@ -5682,7 +5685,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="18" customFormat="1" ht="28">
+    <row r="43" spans="1:17" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>35</v>
       </c>
@@ -5697,7 +5700,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="28">
+    <row r="44" spans="1:17" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -5712,7 +5715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>26</v>
@@ -5733,7 +5736,7 @@
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -5752,7 +5755,7 @@
       <c r="P46" s="21"/>
       <c r="Q46" s="21"/>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>1</v>
       </c>
@@ -5762,7 +5765,9 @@
       <c r="C47" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="22"/>
+      <c r="D47" s="22" t="s">
+        <v>203</v>
+      </c>
       <c r="E47" s="22" t="s">
         <v>5</v>
       </c>
@@ -5779,7 +5784,7 @@
       <c r="P47" s="23"/>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:17" s="21" customFormat="1">
+    <row r="48" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>45</v>
       </c>
@@ -5794,7 +5799,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>45</v>
       </c>
@@ -5808,7 +5813,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="21" customFormat="1">
+    <row r="50" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B50" s="21" t="s">
         <v>49</v>
       </c>
@@ -5816,7 +5821,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D51" s="17" t="s">
         <v>81</v>
       </c>
@@ -5824,7 +5829,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D52" s="17" t="s">
         <v>78</v>
       </c>
@@ -5832,8 +5837,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1"/>
-    <row r="54" spans="1:17" s="39" customFormat="1" ht="28">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:17" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="35" t="s">
         <v>45</v>
       </c>
@@ -5849,7 +5854,7 @@
       </c>
       <c r="G54" s="33"/>
     </row>
-    <row r="55" spans="1:17" ht="28">
+    <row r="55" spans="1:17" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>45</v>
       </c>
@@ -5864,7 +5869,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="26"/>
       <c r="B56" t="s">
         <v>49</v>
@@ -5875,12 +5880,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E57" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -5891,7 +5896,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -5902,7 +5907,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -5921,7 +5926,7 @@
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
         <v>54</v>
       </c>
@@ -5931,15 +5936,10 @@
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5951,7 +5951,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -5959,7 +5959,7 @@
     <col min="4" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="3" customFormat="1" ht="15">
+    <row r="1" spans="1:38" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>96</v>
       </c>
@@ -6001,7 +6001,7 @@
       <c r="AK1" s="11"/>
       <c r="AL1" s="11"/>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
@@ -6049,7 +6049,7 @@
       <c r="AK2" s="11"/>
       <c r="AL2" s="11"/>
     </row>
-    <row r="3" spans="1:38" ht="28">
+    <row r="3" spans="1:38" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -6097,7 +6097,7 @@
       <c r="AK3" s="11"/>
       <c r="AL3" s="11"/>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -6139,7 +6139,7 @@
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
     </row>
-    <row r="5" spans="1:38" s="7" customFormat="1">
+    <row r="5" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -6181,7 +6181,7 @@
       <c r="AK5" s="14"/>
       <c r="AL5" s="14"/>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>6</v>
       </c>
@@ -6195,22 +6195,22 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D7" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D8" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:38" s="7" customFormat="1">
+    <row r="9" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D9" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="43"/>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
@@ -6250,7 +6250,7 @@
       <c r="AK10" s="43"/>
       <c r="AL10" s="43"/>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -6290,7 +6290,7 @@
       <c r="AK11" s="11"/>
       <c r="AL11" s="11"/>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
         <v>1</v>
       </c>
@@ -6338,7 +6338,7 @@
       <c r="AK12" s="11"/>
       <c r="AL12" s="11"/>
     </row>
-    <row r="13" spans="1:38" ht="28">
+    <row r="13" spans="1:38" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>35</v>
       </c>
@@ -6386,7 +6386,7 @@
       <c r="AK13" s="11"/>
       <c r="AL13" s="11"/>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -6428,7 +6428,7 @@
       <c r="AK14" s="11"/>
       <c r="AL14" s="11"/>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -6470,7 +6470,7 @@
       <c r="AK15" s="11"/>
       <c r="AL15" s="11"/>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -6512,7 +6512,7 @@
       <c r="AK16" s="11"/>
       <c r="AL16" s="11"/>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -6552,7 +6552,7 @@
       <c r="AK17" s="11"/>
       <c r="AL17" s="11"/>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" s="42" t="s">
         <v>1</v>
       </c>
@@ -6600,7 +6600,7 @@
       <c r="AK18" s="11"/>
       <c r="AL18" s="11"/>
     </row>
-    <row r="19" spans="1:38" s="21" customFormat="1">
+    <row r="19" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="28">
+    <row r="20" spans="1:38" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
         <v>45</v>
       </c>
@@ -6662,7 +6662,7 @@
       <c r="AK20" s="11"/>
       <c r="AL20" s="11"/>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -6704,7 +6704,7 @@
       <c r="AK21" s="11"/>
       <c r="AL21" s="11"/>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -6746,7 +6746,7 @@
       <c r="AK22" s="11"/>
       <c r="AL22" s="11"/>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -6788,7 +6788,7 @@
       <c r="AK23" s="11"/>
       <c r="AL23" s="11"/>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -6828,7 +6828,7 @@
       <c r="AK24" s="14"/>
       <c r="AL24" s="14"/>
     </row>
-    <row r="25" spans="1:38" s="39" customFormat="1" ht="28">
+    <row r="25" spans="1:38" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
         <v>45</v>
       </c>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="F25" s="33"/>
     </row>
-    <row r="26" spans="1:38" ht="28">
+    <row r="26" spans="1:38" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
         <v>45</v>
       </c>
@@ -6891,7 +6891,7 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="15"/>
@@ -6933,7 +6933,7 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -6975,7 +6975,7 @@
       <c r="AK28" s="11"/>
       <c r="AL28" s="11"/>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -7017,7 +7017,7 @@
       <c r="AK29" s="11"/>
       <c r="AL29" s="11"/>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="43"/>
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
@@ -7060,11 +7060,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7072,24 +7067,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7108,7 +7103,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -7125,7 +7120,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
@@ -7133,17 +7128,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1">
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E6" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -7160,7 +7155,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
@@ -7168,17 +7163,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E10" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -7195,7 +7190,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
@@ -7203,17 +7198,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1">
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E14" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="44" customFormat="1">
+    <row r="15" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -7227,7 +7222,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -7235,13 +7230,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1">
+    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E17" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1"/>
-    <row r="20" spans="1:5" ht="29.25" customHeight="1">
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
         <v>6</v>
       </c>
@@ -7258,7 +7253,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -7269,12 +7264,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="7" customFormat="1">
+    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -7283,7 +7278,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.5" customHeight="1">
+    <row r="24" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -7300,7 +7295,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -7311,7 +7306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>114</v>
       </c>
@@ -7319,7 +7314,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="7" customFormat="1">
+    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -7328,7 +7323,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="18" customFormat="1" ht="32.25" customHeight="1">
+    <row r="28" spans="1:5" s="18" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>6</v>
       </c>
@@ -7343,7 +7338,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="31.5" customHeight="1">
+    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -7358,7 +7353,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="30" spans="1:5" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="14" t="s">
         <v>26</v>
@@ -7367,24 +7362,24 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1">
+    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="43"/>
       <c r="C31" s="43"/>
       <c r="D31" s="43"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1">
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="42" t="s">
         <v>1</v>
       </c>
@@ -7401,7 +7396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.5" customHeight="1">
+    <row r="35" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
         <v>35</v>
       </c>
@@ -7419,7 +7414,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -7430,7 +7425,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -7439,7 +7434,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -7448,7 +7443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -7459,7 +7454,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1">
+    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -7470,7 +7465,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
         <v>35</v>
       </c>
@@ -7485,7 +7480,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" t="s">
         <v>26</v>
@@ -7496,7 +7491,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -7505,7 +7500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -7516,7 +7511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -7527,19 +7522,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="3" customFormat="1">
+    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="43"/>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
       <c r="D46" s="43"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="1:7" ht="28">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
         <v>35</v>
       </c>
@@ -7556,7 +7551,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -7567,12 +7562,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -7581,7 +7576,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -7592,7 +7587,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="7" customFormat="1">
+    <row r="53" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -7603,7 +7598,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="28">
+    <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="35" t="s">
         <v>35</v>
       </c>
@@ -7618,7 +7613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="28">
+    <row r="55" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="35" t="s">
         <v>35</v>
       </c>
@@ -7633,7 +7628,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="7" customFormat="1">
+    <row r="56" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
       <c r="B56" s="7" t="s">
         <v>26</v>
@@ -7642,12 +7637,12 @@
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
     </row>
-    <row r="57" spans="1:15" s="3" customFormat="1">
+    <row r="57" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="43"/>
       <c r="C57" s="43"/>
       <c r="D57" s="43"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -7664,7 +7659,7 @@
       <c r="N58" s="21"/>
       <c r="O58" s="21"/>
     </row>
-    <row r="59" spans="1:15" s="3" customFormat="1">
+    <row r="59" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="42" t="s">
         <v>1</v>
       </c>
@@ -7681,7 +7676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="21" customFormat="1">
+    <row r="60" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>45</v>
       </c>
@@ -7696,7 +7691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="28">
+    <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="35" t="s">
         <v>45</v>
       </c>
@@ -7711,7 +7706,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="11"/>
       <c r="B62" s="11" t="s">
         <v>49</v>
@@ -7722,7 +7717,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -7731,13 +7726,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="7" customFormat="1">
+    <row r="64" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
     </row>
-    <row r="65" spans="1:6" s="21" customFormat="1" ht="28">
+    <row r="65" spans="1:6" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>45</v>
       </c>
@@ -7753,7 +7748,7 @@
       </c>
       <c r="F65" s="39"/>
     </row>
-    <row r="66" spans="1:6" ht="29.25" customHeight="1">
+    <row r="66" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="35" t="s">
         <v>45</v>
       </c>
@@ -7768,7 +7763,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="46"/>
       <c r="B67" s="11" t="s">
         <v>49</v>
@@ -7779,7 +7774,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
@@ -7788,7 +7783,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="11"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -7797,19 +7792,19 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="43"/>
       <c r="B70" s="43"/>
       <c r="C70" s="43"/>
       <c r="D70" s="43"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="27" t="s">
         <v>54</v>
       </c>
@@ -7821,11 +7816,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7837,7 +7827,7 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
@@ -7845,13 +7835,13 @@
     <col min="4" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15">
+    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>128</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7882,7 +7872,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="30.75" customHeight="1">
+    <row r="3" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -7896,7 +7886,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -7904,17 +7894,17 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D5" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="7" customFormat="1">
+    <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D6" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -7928,23 +7918,23 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D8" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D9" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="7" customFormat="1">
+    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D10" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="47" customFormat="1"/>
-    <row r="13" spans="1:21">
+    <row r="11" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -7975,7 +7965,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" s="21" customFormat="1">
+    <row r="14" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
@@ -7989,7 +7979,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="31.5" customHeight="1">
+    <row r="15" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>35</v>
       </c>
@@ -8003,7 +7993,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -8011,7 +8001,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -8019,13 +8009,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="48" customFormat="1"/>
-    <row r="21" spans="1:21">
+    <row r="19" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -8056,7 +8046,7 @@
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
     </row>
-    <row r="22" spans="1:21" s="21" customFormat="1" ht="28">
+    <row r="22" spans="1:21" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>45</v>
       </c>
@@ -8070,7 +8060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="30" customHeight="1">
+    <row r="23" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
         <v>45</v>
       </c>
@@ -8084,7 +8074,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -8092,7 +8082,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -8100,20 +8090,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="7" customFormat="1"/>
+    <row r="28" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8125,7 +8110,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
@@ -8134,13 +8119,13 @@
     <col min="5" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15">
+    <row r="1" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>137</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8172,7 +8157,7 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -8187,7 +8172,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="9"/>
       <c r="C4" s="11"/>
@@ -8196,12 +8181,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="D6" s="5" t="s">
         <v>76</v>
       </c>
@@ -8209,7 +8194,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="7" customFormat="1">
+    <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D7" s="16" t="s">
         <v>78</v>
       </c>
@@ -8217,7 +8202,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8236,7 +8221,7 @@
       <c r="T9" s="44"/>
       <c r="U9" s="44"/>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -8244,7 +8229,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -8255,7 +8240,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -8287,8 +8272,8 @@
       <c r="AC12" s="21"/>
       <c r="AD12" s="21"/>
     </row>
-    <row r="13" spans="1:30" s="7" customFormat="1" ht="17.25" customHeight="1"/>
-    <row r="15" spans="1:30" ht="28">
+    <row r="13" spans="1:30" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>6</v>
       </c>
@@ -8303,7 +8288,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -8312,12 +8297,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D18" s="5" t="s">
         <v>76</v>
       </c>
@@ -8325,7 +8310,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="7" customFormat="1">
+    <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D19" s="16" t="s">
         <v>78</v>
       </c>
@@ -8333,8 +8318,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="21" customFormat="1"/>
-    <row r="21" spans="1:22" s="18" customFormat="1" ht="32.25" customHeight="1">
+    <row r="20" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:22" s="18" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="49" t="s">
         <v>6</v>
       </c>
@@ -8349,7 +8334,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -8381,7 +8366,7 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
         <v>35</v>
       </c>
@@ -8396,7 +8381,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="35"/>
       <c r="B25" s="15"/>
       <c r="C25" s="11"/>
@@ -8405,7 +8390,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -8416,7 +8401,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -8427,7 +8412,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -8436,7 +8421,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -8447,7 +8432,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="7" customFormat="1">
+    <row r="30" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -8458,7 +8443,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
         <v>35</v>
       </c>
@@ -8473,7 +8458,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" t="s">
         <v>26</v>
@@ -8484,7 +8469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -8493,7 +8478,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -8504,7 +8489,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -8515,7 +8500,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -8526,7 +8511,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -8537,7 +8522,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" s="43"/>
       <c r="B38" s="43"/>
       <c r="C38" s="43"/>
@@ -8578,13 +8563,13 @@
       <c r="AL38" s="3"/>
       <c r="AM38" s="3"/>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" spans="1:39" ht="28">
+    <row r="40" spans="1:39" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="s">
         <v>35</v>
       </c>
@@ -8599,12 +8584,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -8613,7 +8598,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -8624,7 +8609,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -8635,7 +8620,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -8646,7 +8631,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:39" s="7" customFormat="1">
+    <row r="46" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -8657,7 +8642,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="28">
+    <row r="47" spans="1:39" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="49" t="s">
         <v>35</v>
       </c>
@@ -8706,7 +8691,7 @@
       <c r="AL47" s="7"/>
       <c r="AM47" s="7"/>
     </row>
-    <row r="48" spans="1:39" ht="28">
+    <row r="48" spans="1:39" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
         <v>35</v>
       </c>
@@ -8721,7 +8706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:39">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
       <c r="B49" s="7" t="s">
         <v>26</v>
@@ -8764,7 +8749,7 @@
       <c r="AL49" s="7"/>
       <c r="AM49" s="7"/>
     </row>
-    <row r="50" spans="1:39">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -8796,7 +8781,7 @@
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
     </row>
-    <row r="51" spans="1:39" s="21" customFormat="1">
+    <row r="51" spans="1:39" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>45</v>
       </c>
@@ -8810,7 +8795,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="28.5" customHeight="1">
+    <row r="52" spans="1:39" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
         <v>45</v>
       </c>
@@ -8825,7 +8810,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" s="11"/>
       <c r="B53" s="11" t="s">
         <v>49</v>
@@ -8836,7 +8821,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:39">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -8845,7 +8830,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:39">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D55" s="5" t="s">
         <v>81</v>
       </c>
@@ -8853,7 +8838,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:39">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D56" s="17" t="s">
         <v>78</v>
       </c>
@@ -8861,13 +8846,13 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:39" s="7" customFormat="1">
+    <row r="57" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
     </row>
-    <row r="58" spans="1:39" s="21" customFormat="1" ht="28">
+    <row r="58" spans="1:39" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>45</v>
       </c>
@@ -8881,7 +8866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:39" ht="29.25" customHeight="1">
+    <row r="59" spans="1:39" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="35" t="s">
         <v>45</v>
       </c>
@@ -8896,7 +8881,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="1:39">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" s="46"/>
       <c r="B60" s="11" t="s">
         <v>49</v>
@@ -8907,7 +8892,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:39">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="11"/>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
@@ -8916,7 +8901,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="62" spans="1:39">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -8925,7 +8910,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="1:39">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D63" s="5" t="s">
         <v>81</v>
       </c>
@@ -8933,7 +8918,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:39">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D64" s="17" t="s">
         <v>78</v>
       </c>
@@ -8941,13 +8926,13 @@
         <v>172</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="3" customFormat="1">
+    <row r="65" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="43"/>
       <c r="B65" s="43"/>
       <c r="C65" s="43"/>
       <c r="D65" s="43"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="27" t="s">
         <v>54</v>
       </c>
@@ -8959,11 +8944,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8975,7 +8955,7 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
@@ -8983,13 +8963,13 @@
     <col min="4" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15">
+    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>173</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9020,7 +9000,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="45.75" customHeight="1">
+    <row r="3" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -9034,7 +9014,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -9042,17 +9022,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D5" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="7" customFormat="1">
+    <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D6" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -9066,22 +9046,22 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D8" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D9" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="7" customFormat="1">
+    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D10" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -9104,7 +9084,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -9135,7 +9115,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="31.5" customHeight="1">
+    <row r="14" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>35</v>
       </c>
@@ -9149,7 +9129,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -9157,7 +9137,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -9165,12 +9145,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -9194,7 +9174,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -9225,7 +9205,7 @@
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:22" ht="30" customHeight="1">
+    <row r="21" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
         <v>45</v>
       </c>
@@ -9239,7 +9219,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -9247,7 +9227,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -9255,12 +9235,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -9287,11 +9267,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9303,147 +9278,147 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="50" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="51" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="50" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="50" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="50" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="50" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>202</v>
       </c>
@@ -9451,10 +9426,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
titles are now groomed with regex
</commit_message>
<xml_diff>
--- a/Backend/app/datasets/app_sug_2.xlsx
+++ b/Backend/app/datasets/app_sug_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="891" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="891" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MDI advice before planned ex" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="204">
   <si>
     <r>
       <rPr>
@@ -1572,7 +1572,7 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4892,8 +4892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4956,9 +4956,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>6</v>
-      </c>
+      <c r="A4" s="31"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="11" t="s">
@@ -4966,9 +4964,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="31"/>
       <c r="D5" s="7" t="s">
         <v>60</v>
       </c>
@@ -4988,25 +4984,19 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="31"/>
       <c r="D7" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="31"/>
       <c r="D8" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
-        <v>6</v>
-      </c>
+      <c r="A9" s="31"/>
       <c r="D9" s="7" t="s">
         <v>66</v>
       </c>
@@ -5239,7 +5229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
parsing the info sheet is done, yet to test and throw it into the json generator function for saving it to file
</commit_message>
<xml_diff>
--- a/Backend/app/datasets/app_sug_2.xlsx
+++ b/Backend/app/datasets/app_sug_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="891" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="891" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="MDI advice before planned ex" sheetId="1" r:id="rId1"/>
@@ -4892,7 +4892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -7058,7 +7058,7 @@
   <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7813,7 +7813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -9262,10 +9262,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9298,118 +9298,118 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="51" t="s">
         <v>181</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="50" t="s">
+        <v>185</v>
+      </c>
+    </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="50" t="s">
-        <v>185</v>
+      <c r="A13" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
         <v>187</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>189</v>
+      </c>
+    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50" t="s">
-        <v>188</v>
+      <c r="A18" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>192</v>
+      <c r="A22" s="50" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50" t="s">
-        <v>193</v>
+      <c r="A23" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
         <v>187</v>
       </c>
     </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="50" t="s">
+        <v>195</v>
+      </c>
+    </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="50" t="s">
-        <v>195</v>
+      <c r="A27" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
         <v>198</v>
       </c>
     </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="50" t="s">
+        <v>199</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="50" t="s">
-        <v>199</v>
+      <c r="A32" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed bg and bg_below_or_... parsing issues. Looking for bugs
</commit_message>
<xml_diff>
--- a/Backend/app/datasets/app_sug_2.xlsx
+++ b/Backend/app/datasets/app_sug_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="891" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="891" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MDI advice before planned ex" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="206">
   <si>
     <r>
       <rPr>
@@ -387,9 +387,6 @@
     <t xml:space="preserve">2. Check blood glucose before you start and at the end of exercise </t>
   </si>
   <si>
-    <t>BG &lt;7</t>
-  </si>
-  <si>
     <t xml:space="preserve">As your blood glucose is &lt; 7mmol/l before you start take 10-30g carbohydrate (amount depends on how much active insulin you have on board) </t>
   </si>
   <si>
@@ -890,12 +887,21 @@
   <si>
     <t>BG</t>
   </si>
+  <si>
+    <t xml:space="preserve">BG below or above target or hypo last 24hrs  </t>
+  </si>
+  <si>
+    <t>BG&lt;7</t>
+  </si>
+  <si>
+    <t>BG&lt;5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -972,6 +978,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1057,10 +1086,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1165,8 +1196,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1572,7 +1608,7 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5229,8 +5265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5258,7 +5294,9 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
@@ -5288,18 +5326,18 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D5" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" t="s">
         <v>76</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D6" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -5317,32 +5355,29 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D10" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" t="s">
         <v>81</v>
-      </c>
-      <c r="E10" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D11" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -5374,35 +5409,35 @@
         <v>6</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D16" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" t="s">
         <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D17" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="30" x14ac:dyDescent="0.2">
@@ -5449,9 +5484,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -5500,14 +5533,14 @@
         <v>35</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R24" s="18"/>
       <c r="S24" s="18"/>
@@ -5519,7 +5552,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
@@ -5534,10 +5567,10 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E26" t="s">
         <v>76</v>
-      </c>
-      <c r="E26" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
@@ -5545,24 +5578,20 @@
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D28" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D28" s="17"/>
       <c r="E28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D29" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="D29" s="16"/>
       <c r="E29" s="7" t="s">
         <v>39</v>
       </c>
@@ -5591,7 +5620,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -5599,10 +5628,10 @@
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="5" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -5610,10 +5639,10 @@
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="D34" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -5622,19 +5651,19 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
@@ -5642,10 +5671,10 @@
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="17" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="E39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
@@ -5653,24 +5682,20 @@
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D41" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D41" s="53"/>
       <c r="E41" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D42" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D42" s="53"/>
       <c r="E42" s="7" t="s">
         <v>39</v>
       </c>
@@ -5756,7 +5781,7 @@
         <v>3</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E47" s="22" t="s">
         <v>5</v>
@@ -5804,27 +5829,24 @@
       </c>
     </row>
     <row r="50" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="21" t="s">
-        <v>49</v>
-      </c>
       <c r="E50" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D51" s="17" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D52" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -5856,14 +5878,11 @@
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="26"/>
-      <c r="B56" t="s">
-        <v>49</v>
-      </c>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="11" t="s">
@@ -5872,7 +5891,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -5880,10 +5899,10 @@
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
       <c r="D58" s="17" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
@@ -5891,10 +5910,10 @@
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
       <c r="D59" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
@@ -5951,7 +5970,7 @@
   <sheetData>
     <row r="1" spans="1:38" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="11"/>
@@ -6339,7 +6358,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -6615,7 +6634,7 @@
         <v>62</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -6844,7 +6863,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -7070,7 +7089,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -7085,7 +7104,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -7107,7 +7126,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -7115,7 +7134,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7125,7 +7144,7 @@
     </row>
     <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7142,7 +7161,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7150,7 +7169,7 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -7160,7 +7179,7 @@
     </row>
     <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E10" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7177,7 +7196,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -7185,7 +7204,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -7195,7 +7214,7 @@
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E14" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -7209,7 +7228,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -7217,12 +7236,12 @@
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E17" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -7240,7 +7259,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -7251,7 +7270,7 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -7265,7 +7284,7 @@
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -7282,7 +7301,7 @@
         <v>9</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -7293,12 +7312,12 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
         <v>31</v>
@@ -7310,7 +7329,7 @@
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="18" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7380,7 +7399,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>5</v>
@@ -7391,7 +7410,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>8</v>
@@ -7400,7 +7419,7 @@
         <v>9</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G35" s="11"/>
     </row>
@@ -7412,7 +7431,7 @@
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -7421,7 +7440,7 @@
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -7467,7 +7486,7 @@
       </c>
       <c r="D41" s="11"/>
       <c r="E41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -7529,7 +7548,7 @@
         <v>35</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>29</v>
@@ -7538,7 +7557,7 @@
         <v>9</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
@@ -7549,12 +7568,12 @@
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -7563,7 +7582,7 @@
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
       <c r="E51" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -7660,7 +7679,7 @@
         <v>3</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>5</v>
@@ -7693,7 +7712,7 @@
       </c>
       <c r="D61" s="11"/>
       <c r="E61" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
@@ -7704,7 +7723,7 @@
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
@@ -7750,7 +7769,7 @@
       </c>
       <c r="D66" s="11"/>
       <c r="E66" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -7761,7 +7780,7 @@
       <c r="C67" s="15"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -7770,7 +7789,7 @@
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -7779,7 +7798,7 @@
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7827,7 +7846,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -7873,7 +7892,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -7881,7 +7900,7 @@
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -7891,7 +7910,7 @@
     </row>
     <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D6" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -7905,7 +7924,7 @@
         <v>62</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -7920,7 +7939,7 @@
     </row>
     <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D10" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -7974,13 +7993,13 @@
         <v>35</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
@@ -8001,7 +8020,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -8061,7 +8080,7 @@
         <v>57</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
@@ -8082,7 +8101,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -8096,8 +8115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8111,7 +8130,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -8125,7 +8144,9 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
@@ -8159,7 +8180,7 @@
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -8168,28 +8189,28 @@
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="E6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D7" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -8204,7 +8225,7 @@
       </c>
       <c r="D9" s="44"/>
       <c r="E9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R9" s="44"/>
       <c r="S9" s="44"/>
@@ -8216,7 +8237,7 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
@@ -8224,10 +8245,10 @@
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="5" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
@@ -8235,10 +8256,10 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -8268,14 +8289,14 @@
         <v>6</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
@@ -8284,28 +8305,28 @@
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D18" s="5" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D19" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -8314,14 +8335,14 @@
         <v>6</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="37" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="37"/>
       <c r="E21" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
@@ -8368,7 +8389,7 @@
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
@@ -8377,29 +8398,25 @@
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
-      <c r="D26" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D26" s="52"/>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D27" s="52"/>
       <c r="E27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
@@ -8408,7 +8425,7 @@
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -8416,10 +8433,10 @@
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="5" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="E29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8427,10 +8444,10 @@
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -8445,7 +8462,7 @@
       </c>
       <c r="D31" s="11"/>
       <c r="E31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -8465,29 +8482,25 @@
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D34" s="53"/>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D35" s="53"/>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.2">
@@ -8495,10 +8508,10 @@
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="5" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.2">
@@ -8506,10 +8519,10 @@
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.2">
@@ -8564,19 +8577,19 @@
         <v>35</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.2">
@@ -8585,7 +8598,7 @@
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.2">
@@ -8593,10 +8606,10 @@
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="D43" s="5" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="E43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.2">
@@ -8604,32 +8617,28 @@
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
-      <c r="D45" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D45" s="53"/>
       <c r="E45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
-      <c r="D46" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="D46" s="54"/>
       <c r="E46" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:39" ht="30" x14ac:dyDescent="0.2">
@@ -8797,7 +8806,7 @@
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.2">
@@ -8808,7 +8817,7 @@
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.2">
@@ -8817,23 +8826,23 @@
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D55" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D56" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8868,7 +8877,7 @@
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.2">
@@ -8879,7 +8888,7 @@
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
       <c r="E60" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.2">
@@ -8888,7 +8897,7 @@
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.2">
@@ -8897,23 +8906,23 @@
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D63" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D64" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -8955,7 +8964,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -9001,7 +9010,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -9014,12 +9023,12 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D5" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D6" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -9033,7 +9042,7 @@
         <v>62</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -9048,7 +9057,7 @@
     </row>
     <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D10" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -9110,13 +9119,13 @@
         <v>35</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>57</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
@@ -9137,7 +9146,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -9206,7 +9215,7 @@
         <v>57</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -9227,7 +9236,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
@@ -9264,7 +9273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -9275,142 +9284,142 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="50" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue where the last item was being popped from exercise types as the schema was not consistent throughout the sheets
</commit_message>
<xml_diff>
--- a/Backend/app/datasets/app_sug_2.xlsx
+++ b/Backend/app/datasets/app_sug_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="891" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="891"/>
   </bookViews>
   <sheets>
     <sheet name="MDI advice before planned ex" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="207">
   <si>
     <r>
       <rPr>
@@ -895,6 +895,9 @@
   </si>
   <si>
     <t>BG&lt;5</t>
+  </si>
+  <si>
+    <t>moderate/intense/extremely intense</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1089,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1200,9 +1205,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1607,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1965,17 +1972,13 @@
       </c>
     </row>
     <row r="38" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="D38" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="D38" s="5"/>
       <c r="E38" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D39" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="D39" s="16"/>
       <c r="E39" s="7" t="s">
         <v>39</v>
       </c>
@@ -4753,17 +4756,13 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D49" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D49" s="17"/>
       <c r="E49" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D50" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="D50" s="17"/>
       <c r="E50" t="s">
         <v>39</v>
       </c>
@@ -4926,10 +4925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5255,6 +5254,11 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5265,8 +5269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5954,10 +5958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL30"/>
+  <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7066,6 +7070,11 @@
       <c r="AK30" s="11"/>
       <c r="AL30" s="11"/>
     </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A32" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7076,7 +7085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -7830,10 +7839,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7988,26 +7997,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+    <row r="15" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B16" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -8015,15 +8017,25 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
+    <row r="19" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>1</v>
@@ -8069,26 +8081,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+    <row r="23" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="B24" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
@@ -8096,15 +8101,29 @@
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:21" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8115,7 +8134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -8948,10 +8967,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9263,6 +9282,11 @@
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
     </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>